<commit_message>
Funcoes alteradas para atualizar resultados antes de atender a chamada do usuario e estruta de arquivos alterada para separar funcoes nao exportadas
</commit_message>
<xml_diff>
--- a/data-raw/resultados_diadesorte.xlsx
+++ b/data-raw/resultados_diadesorte.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4579"/>
+  <dimension ref="A1:E4586"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -78217,6 +78217,125 @@
         <v>27</v>
       </c>
     </row>
+    <row r="4580">
+      <c r="A4580" s="2">
+        <v>44817</v>
+      </c>
+      <c r="B4580">
+        <v>655</v>
+      </c>
+      <c r="C4580">
+        <v>0</v>
+      </c>
+      <c r="D4580">
+        <v>0</v>
+      </c>
+      <c r="E4580">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4581">
+      <c r="A4581" s="2">
+        <v>44817</v>
+      </c>
+      <c r="B4581">
+        <v>655</v>
+      </c>
+      <c r="C4581">
+        <v>0</v>
+      </c>
+      <c r="D4581">
+        <v>0</v>
+      </c>
+      <c r="E4581">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4582">
+      <c r="A4582" s="2">
+        <v>44817</v>
+      </c>
+      <c r="B4582">
+        <v>655</v>
+      </c>
+      <c r="C4582">
+        <v>0</v>
+      </c>
+      <c r="D4582">
+        <v>0</v>
+      </c>
+      <c r="E4582">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4583">
+      <c r="A4583" s="2">
+        <v>44817</v>
+      </c>
+      <c r="B4583">
+        <v>655</v>
+      </c>
+      <c r="C4583">
+        <v>0</v>
+      </c>
+      <c r="D4583">
+        <v>0</v>
+      </c>
+      <c r="E4583">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4584">
+      <c r="A4584" s="2">
+        <v>44817</v>
+      </c>
+      <c r="B4584">
+        <v>655</v>
+      </c>
+      <c r="C4584">
+        <v>0</v>
+      </c>
+      <c r="D4584">
+        <v>0</v>
+      </c>
+      <c r="E4584">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4585">
+      <c r="A4585" s="2">
+        <v>44817</v>
+      </c>
+      <c r="B4585">
+        <v>655</v>
+      </c>
+      <c r="C4585">
+        <v>0</v>
+      </c>
+      <c r="D4585">
+        <v>0</v>
+      </c>
+      <c r="E4585">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4586">
+      <c r="A4586" s="2">
+        <v>44817</v>
+      </c>
+      <c r="B4586">
+        <v>655</v>
+      </c>
+      <c r="C4586">
+        <v>0</v>
+      </c>
+      <c r="D4586">
+        <v>0</v>
+      </c>
+      <c r="E4586">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajustes para verificar se houve ganhador
</commit_message>
<xml_diff>
--- a/data-raw/resultados_diadesorte.xlsx
+++ b/data-raw/resultados_diadesorte.xlsx
@@ -78344,7 +78344,7 @@
         <v>656</v>
       </c>
       <c r="C4587">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4587">
         <v>0</v>
@@ -78361,7 +78361,7 @@
         <v>656</v>
       </c>
       <c r="C4588">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4588">
         <v>0</v>
@@ -78378,7 +78378,7 @@
         <v>656</v>
       </c>
       <c r="C4589">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4589">
         <v>0</v>
@@ -78395,7 +78395,7 @@
         <v>656</v>
       </c>
       <c r="C4590">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4590">
         <v>0</v>
@@ -78412,7 +78412,7 @@
         <v>656</v>
       </c>
       <c r="C4591">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4591">
         <v>0</v>
@@ -78429,7 +78429,7 @@
         <v>656</v>
       </c>
       <c r="C4592">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4592">
         <v>0</v>
@@ -78446,7 +78446,7 @@
         <v>656</v>
       </c>
       <c r="C4593">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4593">
         <v>0</v>

</xml_diff>